<commit_message>
new noise trackers, using MATHS
</commit_message>
<xml_diff>
--- a/data/playtesting.xlsx
+++ b/data/playtesting.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sessions" sheetId="2" r:id="rId1"/>
-    <sheet name="The Greedy Prisoner - Aug 3" sheetId="1" r:id="rId2"/>
-    <sheet name="Greedy Prisoner - Aug 4, 4P" sheetId="3" r:id="rId3"/>
+    <sheet name="GreedyP - Aug 3" sheetId="1" r:id="rId2"/>
+    <sheet name="GreedyP - Aug 4, 4P" sheetId="3" r:id="rId3"/>
+    <sheet name="GreedyP - Aug 5" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="70">
   <si>
     <t>Date</t>
   </si>
@@ -205,6 +206,27 @@
   </si>
   <si>
     <t>Thug+Pilfer+Hurry</t>
+  </si>
+  <si>
+    <t>Noise/Rnd/Player</t>
+  </si>
+  <si>
+    <t>Security Handled</t>
+  </si>
+  <si>
+    <t>Team Avg Level</t>
+  </si>
+  <si>
+    <t>Game Version</t>
+  </si>
+  <si>
+    <t># Events</t>
+  </si>
+  <si>
+    <t>Alerts from Events</t>
+  </si>
+  <si>
+    <t>Alerts from Event</t>
   </si>
 </sst>
 </file>
@@ -266,7 +288,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -299,11 +321,26 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -609,10 +646,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W5"/>
+  <dimension ref="A1:AC6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -621,116 +658,145 @@
     <col min="2" max="2" width="8.7265625" style="6"/>
     <col min="3" max="3" width="16.7265625" style="6" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="8.7265625" style="6"/>
-    <col min="6" max="6" width="17.90625" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.1796875" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.453125" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="31.81640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.7265625" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="27.7265625" style="6" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.7265625" style="6" bestFit="1" customWidth="1"/>
-    <col min="13" max="22" width="8.7265625" style="6"/>
-    <col min="23" max="16384" width="8.7265625" style="5"/>
+    <col min="6" max="6" width="15.6328125" style="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.54296875" style="12" customWidth="1"/>
+    <col min="8" max="8" width="12" style="12" customWidth="1"/>
+    <col min="9" max="9" width="7.1796875" style="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="7.54296875" style="12" customWidth="1"/>
+    <col min="12" max="12" width="17.90625" style="6" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.1796875" style="6" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="24.453125" style="6" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="31.81640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.7265625" style="6" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="27.7265625" style="6" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.7265625" style="6" bestFit="1" customWidth="1"/>
+    <col min="19" max="28" width="8.7265625" style="6"/>
+    <col min="29" max="16384" width="8.7265625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:29" s="10" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="H1" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="I1" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="J1" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="K1" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="L1" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="M1" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="N1" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="O1" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="P1" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="Q1" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="L1" s="12" t="s">
+      <c r="R1" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
-      <c r="O1" s="12"/>
-      <c r="P1" s="12"/>
-      <c r="Q1" s="12"/>
-      <c r="R1" s="12"/>
-      <c r="S1" s="12"/>
-      <c r="T1" s="12"/>
-      <c r="U1" s="12"/>
-      <c r="V1" s="12" t="s">
+      <c r="S1" s="13"/>
+      <c r="T1" s="13"/>
+      <c r="U1" s="13"/>
+      <c r="V1" s="13"/>
+      <c r="W1" s="13"/>
+      <c r="X1" s="13"/>
+      <c r="Y1" s="13"/>
+      <c r="Z1" s="13"/>
+      <c r="AA1" s="13"/>
+      <c r="AB1" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="W1" s="12" t="s">
+      <c r="AC1" s="13" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:23" s="8" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="13"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9" t="s">
+    <row r="2" spans="1:29" s="8" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="14"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="9"/>
+      <c r="O2" s="9"/>
+      <c r="P2" s="9"/>
+      <c r="Q2" s="9"/>
+      <c r="R2" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="M2" s="9" t="s">
+      <c r="S2" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="9" t="s">
+      <c r="T2" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="O2" s="9" t="s">
+      <c r="U2" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="P2" s="9" t="s">
+      <c r="V2" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="Q2" s="9" t="s">
+      <c r="W2" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="R2" s="9" t="s">
+      <c r="X2" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="S2" s="9" t="s">
+      <c r="Y2" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="T2" s="9" t="s">
+      <c r="Z2" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="U2" s="9" t="s">
+      <c r="AA2" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="V2" s="13"/>
-      <c r="W2" s="13"/>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="AB2" s="14"/>
+      <c r="AC2" s="14"/>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A3" s="7">
         <v>44035</v>
       </c>
@@ -746,42 +812,55 @@
       <c r="E3" s="6">
         <v>28</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="12">
+        <f>(E3/D3)/B3</f>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="H3" s="12">
+        <v>1</v>
+      </c>
+      <c r="I3" s="12">
+        <v>18</v>
+      </c>
+      <c r="J3" s="12">
+        <v>24</v>
+      </c>
+      <c r="L3" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="M3" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="L3" s="6">
+      <c r="R3" s="6">
         <v>27</v>
       </c>
-      <c r="M3" s="6">
+      <c r="S3" s="6">
         <v>16</v>
       </c>
-      <c r="N3" s="6">
+      <c r="T3" s="6">
         <v>9</v>
       </c>
-      <c r="O3" s="6">
+      <c r="U3" s="6">
         <v>10</v>
       </c>
-      <c r="P3" s="6">
+      <c r="V3" s="6">
         <v>15</v>
       </c>
-      <c r="Q3" s="6">
+      <c r="W3" s="6">
         <v>7</v>
       </c>
-      <c r="R3" s="6">
+      <c r="X3" s="6">
         <v>7</v>
       </c>
-      <c r="S3" s="6">
+      <c r="Y3" s="6">
         <v>8</v>
       </c>
-      <c r="V3" s="6">
-        <f>SUM(L3:U3)</f>
+      <c r="AB3" s="6">
+        <f>SUM(R3:AA3)</f>
         <v>99</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A4" s="7">
         <v>44046</v>
       </c>
@@ -797,26 +876,39 @@
       <c r="E4" s="6">
         <v>43</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="12">
+        <f t="shared" ref="F4:F5" si="0">(E4/D4)/B4</f>
+        <v>1.5925925925925926</v>
+      </c>
+      <c r="H4" s="12">
+        <v>2</v>
+      </c>
+      <c r="I4" s="12">
+        <v>19</v>
+      </c>
+      <c r="J4" s="12">
+        <v>24</v>
+      </c>
+      <c r="L4" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="M4" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="N4" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="I4" s="6" t="s">
+      <c r="O4" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="J4" s="6" t="s">
+      <c r="P4" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="W4" s="5" t="s">
+      <c r="AC4" s="5" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A5" s="7">
         <v>44047</v>
       </c>
@@ -832,42 +924,88 @@
       <c r="E5" s="6">
         <v>39</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="12">
+        <f t="shared" si="0"/>
+        <v>1.21875</v>
+      </c>
+      <c r="G5" s="12">
+        <v>14</v>
+      </c>
+      <c r="H5" s="12">
+        <v>2</v>
+      </c>
+      <c r="I5" s="12">
+        <v>19</v>
+      </c>
+      <c r="J5" s="12">
+        <v>24</v>
+      </c>
+      <c r="L5" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="M5" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="N5" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="I5" s="6" t="s">
+      <c r="O5" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="J5" s="6" t="s">
+      <c r="P5" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="K5" s="6" t="s">
+      <c r="Q5" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="W5" s="5" t="s">
+      <c r="AC5" s="5" t="s">
         <v>59</v>
       </c>
     </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="A6" s="7">
+        <v>44048</v>
+      </c>
+      <c r="B6" s="6">
+        <v>4</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="12">
+        <v>2</v>
+      </c>
+      <c r="I6" s="12">
+        <v>19</v>
+      </c>
+      <c r="J6" s="12">
+        <v>24</v>
+      </c>
+      <c r="L6" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="16">
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:D2"/>
-    <mergeCell ref="W1:W2"/>
+    <mergeCell ref="AC1:AC2"/>
+    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="AB1:AB2"/>
+    <mergeCell ref="R1:AA1"/>
+    <mergeCell ref="F1:F2"/>
     <mergeCell ref="G1:G2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="V1:V2"/>
-    <mergeCell ref="L1:U1"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="K1:K2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -875,8 +1013,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1083,8 +1221,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1262,4 +1400,153 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="2" width="8.7265625" style="4"/>
+    <col min="3" max="3" width="10.36328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7265625" style="4"/>
+    <col min="5" max="5" width="15.26953125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.7265625" style="4"/>
+    <col min="7" max="7" width="15.6328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="3">
+        <v>44048</v>
+      </c>
+      <c r="B2" s="4">
+        <v>1</v>
+      </c>
+      <c r="H2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" s="3">
+        <v>44048</v>
+      </c>
+      <c r="B3" s="4">
+        <v>2</v>
+      </c>
+      <c r="H3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" s="3">
+        <v>44048</v>
+      </c>
+      <c r="B4" s="4">
+        <v>3</v>
+      </c>
+      <c r="H4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" s="3">
+        <v>44048</v>
+      </c>
+      <c r="B5" s="4">
+        <v>4</v>
+      </c>
+      <c r="H5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" s="3">
+        <v>44048</v>
+      </c>
+      <c r="B6" s="4">
+        <v>5</v>
+      </c>
+      <c r="H6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" s="3">
+        <v>44048</v>
+      </c>
+      <c r="B7" s="4">
+        <v>6</v>
+      </c>
+      <c r="H7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" s="3">
+        <v>44048</v>
+      </c>
+      <c r="B8" s="4">
+        <v>7</v>
+      </c>
+      <c r="H8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" s="3">
+        <v>44048</v>
+      </c>
+      <c r="B9" s="4">
+        <v>8</v>
+      </c>
+      <c r="H9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" s="3">
+        <v>44048</v>
+      </c>
+      <c r="B10" s="4">
+        <v>9</v>
+      </c>
+      <c r="H10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>